<commit_message>
Completion of unit testing for S3, MetaProcess and XetraTransformer
</commit_message>
<xml_diff>
--- a/tests/Test_Specification.xlsx
+++ b/tests/Test_Specification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kira_\VSCode\py_etl\xetra_1234\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665705CA-6B69-4752-AE23-C12AB7C69187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6DEFEC-CB38-4208-9EF6-5B60E438A85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D343E84-D58A-4425-9255-64B4AEA8C315}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>module</t>
   </si>
@@ -95,6 +95,55 @@
   </si>
   <si>
     <t>empty list</t>
+  </si>
+  <si>
+    <t>read_csv_to_df</t>
+  </si>
+  <si>
+    <t>Test the read_csv_to_df method for reading 1 .csv file from the mocked s3 bucket</t>
+  </si>
+  <si>
+    <t>test_read_csv_to_df_ok</t>
+  </si>
+  <si>
+    <t>Test the write_df_to_s3 method within an empty DataFrame as input</t>
+  </si>
+  <si>
+    <t>test_write_df_to_s3_empty</t>
+  </si>
+  <si>
+    <t>write_df_to_s3</t>
+  </si>
+  <si>
+    <t>test.csv</t>
+  </si>
+  <si>
+    <t>empty DataFrame</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>DataFrame with the content of the csv file</t>
+  </si>
+  <si>
+    <t>Mock s3 bucket
+Read csv file from it into DataFrame</t>
+  </si>
+  <si>
+    <t>test_write_df_to_s3_parquet</t>
+  </si>
+  <si>
+    <t>test_write_df_to_s3_csv</t>
+  </si>
+  <si>
+    <t>Tests if writting a csv file to write_df_to_s3 method succeeds</t>
+  </si>
+  <si>
+    <t>Tests if writting a parquet file to write_df_to_s3 method succeeds</t>
+  </si>
+  <si>
+    <t>test.parquet</t>
   </si>
 </sst>
 </file>
@@ -181,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -195,6 +244,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,11 +561,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9C9B1C-5DCA-46BB-97EA-EA14CB33724B}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +575,7 @@
     <col min="3" max="3" width="37.21875" style="6" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" style="7" customWidth="1"/>
     <col min="5" max="5" width="36.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.5546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
@@ -594,6 +646,83 @@
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integration test + Piplock
</commit_message>
<xml_diff>
--- a/tests/Test_Specification.xlsx
+++ b/tests/Test_Specification.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kira_\VSCode\py_etl\xetra_1234\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6DEFEC-CB38-4208-9EF6-5B60E438A85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B4C363-7BDB-403B-907E-2B08936D8383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D343E84-D58A-4425-9255-64B4AEA8C315}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5D343E84-D58A-4425-9255-64B4AEA8C315}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Unit Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Integration Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Integration Test'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Unit Test'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>module</t>
   </si>
@@ -144,6 +146,22 @@
   </si>
   <si>
     <t>test.parquet</t>
+  </si>
+  <si>
+    <t>test_int_etl_report_no_metafile</t>
+  </si>
+  <si>
+    <t>Integration test for the main entrypoint etl_report1</t>
+  </si>
+  <si>
+    <t>s3 source bucket with source content
+Create S3BucketConnector test instance</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>.parquet file on s3 with the source data content in report 1 format</t>
   </si>
 </sst>
 </file>
@@ -230,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -247,6 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9C9B1C-5DCA-46BB-97EA-EA14CB33724B}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
@@ -730,4 +749,70 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383B0ACD-F5F0-410D-88DB-E00A867E4E92}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="7"/>
+      <c r="E4" s="9"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{9C9C9B1C-5DCA-46BB-97EA-EA14CB33724B}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>